<commit_message>
Enhance Excel report generation and update .gitignore: - Introduce a new function to find image paths based on account number and DIN, improving image retrieval logic. - Update hyperlinks in the Excel report to reference the new "Detail Data" sheet instead of "Raw Data". - Modify .gitignore to exclude generated fake data and Excel files, ensuring cleaner repository management.
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Summary Table" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Raw Data" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Detail Data" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Images" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
@@ -2157,7 +2157,7 @@
     <row r="1">
       <c r="B1" t="inlineStr">
         <is>
-          <t>Raw Fake Data</t>
+          <t>Detail Data</t>
         </is>
       </c>
     </row>

</xml_diff>